<commit_message>
Finished replication of excel
</commit_message>
<xml_diff>
--- a/doc/import_vendor_list.xlsx
+++ b/doc/import_vendor_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="501" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="250" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="127">
   <si>
     <t>Item</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Carbonless Forms</t>
   </si>
   <si>
-    <t>expensive</t>
-  </si>
-  <si>
     <t>Enter To Win Pad</t>
   </si>
   <si>
@@ -327,46 +324,25 @@
     <t>4x6 Stock Paper (4/0, qty 250)</t>
   </si>
   <si>
-    <t> / 36.00</t>
-  </si>
-  <si>
     <t>4x6 Stock Paper (4/4, qty 250)</t>
   </si>
   <si>
-    <t>49.00 / 45.00</t>
-  </si>
-  <si>
     <t>4x6 Stock Paper (4/0, qty 500)</t>
   </si>
   <si>
-    <t> /  </t>
-  </si>
-  <si>
     <t>4x6 Stock Paper (4/4, qty 500)</t>
   </si>
   <si>
     <t>4x6 Stock Paper (4/0, qty 1000)</t>
   </si>
   <si>
-    <t> / 65.00</t>
-  </si>
-  <si>
     <t>4x6 Stock Paper (4/4, qty 1000)</t>
   </si>
   <si>
-    <t> / 120.00</t>
-  </si>
-  <si>
     <t>4x6 Stock Paper (4/0, qty 2500)</t>
   </si>
   <si>
-    <t> / 125.00</t>
-  </si>
-  <si>
     <t>4x6 Stock Paper (4/4, qty 2500)</t>
-  </si>
-  <si>
-    <t> / 225.00</t>
   </si>
   <si>
     <t>4x6 Stock Paper (4/0, qty 5000)</t>
@@ -711,9 +687,9 @@
   <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A113" activeCellId="0" sqref="A113"/>
+      <selection pane="bottomLeft" activeCell="D83" activeCellId="0" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1277,9 +1253,7 @@
         <v>35</v>
       </c>
       <c r="C22" s="18"/>
-      <c r="D22" s="18" t="s">
-        <v>36</v>
-      </c>
+      <c r="D22" s="18"/>
       <c r="E22" s="3" t="s">
         <v>11</v>
       </c>
@@ -1296,10 +1270,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>38</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>11</v>
@@ -1323,10 +1297,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="18" t="n">
         <v>105</v>
@@ -1348,10 +1322,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>41</v>
       </c>
       <c r="C25" s="18" t="n">
         <v>34</v>
@@ -1371,10 +1345,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>11</v>
@@ -1394,10 +1368,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="20" t="n">
         <v>58</v>
@@ -1419,10 +1393,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="19"/>
@@ -1440,10 +1414,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="21" t="n">
         <v>58</v>
@@ -1465,10 +1439,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>11</v>
@@ -1488,10 +1462,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>11</v>
@@ -1511,10 +1485,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="19" t="n">
         <v>216</v>
@@ -1534,10 +1508,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="17" t="n">
         <v>87</v>
@@ -1559,10 +1533,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="17" t="n">
         <v>117</v>
@@ -1584,10 +1558,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>11</v>
@@ -1609,10 +1583,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>11</v>
@@ -1634,10 +1608,10 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>11</v>
@@ -1657,10 +1631,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>11</v>
@@ -1680,10 +1654,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>11</v>
@@ -1703,10 +1677,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>11</v>
@@ -1728,10 +1702,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" s="18" t="n">
         <v>98</v>
@@ -1753,10 +1727,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" s="20" t="n">
         <v>98</v>
@@ -1776,10 +1750,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="20" t="n">
         <v>118</v>
@@ -1799,10 +1773,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="18" t="n">
         <v>118</v>
@@ -1822,10 +1796,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -1843,10 +1817,10 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -1864,10 +1838,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
@@ -1885,10 +1859,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>11</v>
@@ -1914,10 +1888,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>11</v>
@@ -1943,10 +1917,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>11</v>
@@ -1972,10 +1946,10 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="23" t="s">
         <v>67</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>68</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>11</v>
@@ -2001,10 +1975,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C52" s="18" t="n">
         <v>43</v>
@@ -2026,10 +2000,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>11</v>
@@ -2053,10 +2027,10 @@
     </row>
     <row r="54" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C54" s="17" t="n">
         <v>52</v>
@@ -2080,10 +2054,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C55" s="19" t="n">
         <v>67</v>
@@ -2107,10 +2081,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C56" s="17" t="n">
         <v>74</v>
@@ -2134,10 +2108,10 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C57" s="17" t="n">
         <v>78</v>
@@ -2159,10 +2133,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C58" s="17" t="n">
         <v>88</v>
@@ -2184,10 +2158,10 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C59" s="18" t="s">
         <v>11</v>
@@ -2211,10 +2185,10 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>11</v>
@@ -2238,10 +2212,10 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="18" t="s">
         <v>11</v>
@@ -2265,10 +2239,10 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C62" s="18" t="s">
         <v>11</v>
@@ -2292,10 +2266,10 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C63" s="18" t="s">
         <v>11</v>
@@ -2319,10 +2293,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C64" s="18"/>
       <c r="D64" s="3"/>
@@ -2344,10 +2318,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C65" s="19" t="n">
         <v>159</v>
@@ -2373,10 +2347,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C66" s="19" t="n">
         <v>193</v>
@@ -2398,10 +2372,10 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67" s="16" t="s">
         <v>84</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>85</v>
       </c>
       <c r="C67" s="18" t="n">
         <v>76</v>
@@ -2423,10 +2397,10 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C68" s="18" t="n">
         <v>98</v>
@@ -2450,10 +2424,10 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C69" s="17" t="n">
         <v>54</v>
@@ -2475,17 +2449,15 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C70" s="17" t="n">
         <v>73</v>
       </c>
-      <c r="D70" s="18" t="s">
-        <v>36</v>
-      </c>
+      <c r="D70" s="18"/>
       <c r="E70" s="18"/>
       <c r="F70" s="18" t="s">
         <v>11</v>
@@ -2502,10 +2474,10 @@
     </row>
     <row r="71" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="23" t="s">
         <v>89</v>
-      </c>
-      <c r="B71" s="23" t="s">
-        <v>90</v>
       </c>
       <c r="C71" s="19" t="n">
         <v>74</v>
@@ -2527,10 +2499,10 @@
     </row>
     <row r="72" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C72" s="19" t="n">
         <v>134</v>
@@ -2554,10 +2526,10 @@
     </row>
     <row r="73" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C73" s="19" t="n">
         <v>216</v>
@@ -2579,10 +2551,10 @@
     </row>
     <row r="74" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C74" s="19" t="s">
         <v>11</v>
@@ -2606,10 +2578,10 @@
     </row>
     <row r="75" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C75" s="19" t="n">
         <v>408</v>
@@ -2633,10 +2605,10 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" s="19" t="s">
         <v>11</v>
@@ -2658,10 +2630,10 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="B77" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="C77" s="17" t="n">
         <v>55</v>
@@ -2685,10 +2657,10 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" s="17" t="n">
         <v>82</v>
@@ -2710,10 +2682,10 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" s="17" t="n">
         <v>55</v>
@@ -2737,10 +2709,10 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C80" s="15" t="n">
         <v>15</v>
@@ -2762,17 +2734,15 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" s="24" t="s">
         <v>101</v>
-      </c>
-      <c r="B81" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="C81" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="D81" s="22" t="s">
-        <v>103</v>
-      </c>
+      <c r="D81" s="22"/>
       <c r="E81" s="19" t="n">
         <v>20</v>
       </c>
@@ -2791,17 +2761,15 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C82" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="D82" s="22" t="s">
-        <v>105</v>
-      </c>
+      <c r="D82" s="22"/>
       <c r="E82" s="19" t="n">
         <v>35</v>
       </c>
@@ -2820,15 +2788,13 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C83" s="22"/>
-      <c r="D83" s="22" t="s">
-        <v>107</v>
-      </c>
+      <c r="D83" s="22"/>
       <c r="E83" s="22"/>
       <c r="F83" s="18" t="s">
         <v>11</v>
@@ -2845,15 +2811,13 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C84" s="22"/>
-      <c r="D84" s="22" t="s">
-        <v>107</v>
-      </c>
+      <c r="D84" s="22"/>
       <c r="E84" s="22"/>
       <c r="F84" s="18" t="s">
         <v>11</v>
@@ -2870,15 +2834,13 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C85" s="22"/>
-      <c r="D85" s="22" t="s">
-        <v>110</v>
-      </c>
+      <c r="D85" s="22"/>
       <c r="E85" s="22" t="n">
         <v>68</v>
       </c>
@@ -2897,15 +2859,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C86" s="22"/>
-      <c r="D86" s="22" t="s">
-        <v>112</v>
-      </c>
+      <c r="D86" s="22"/>
       <c r="E86" s="22" t="n">
         <v>115</v>
       </c>
@@ -2924,15 +2884,13 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C87" s="22"/>
-      <c r="D87" s="22" t="s">
-        <v>114</v>
-      </c>
+      <c r="D87" s="22"/>
       <c r="E87" s="22" t="n">
         <v>118</v>
       </c>
@@ -2951,17 +2909,15 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C88" s="22" t="n">
         <v>58</v>
       </c>
-      <c r="D88" s="22" t="s">
-        <v>116</v>
-      </c>
+      <c r="D88" s="22"/>
       <c r="E88" s="22" t="n">
         <v>139</v>
       </c>
@@ -2980,15 +2936,13 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B89" s="24" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C89" s="22"/>
-      <c r="D89" s="22" t="s">
-        <v>107</v>
-      </c>
+      <c r="D89" s="22"/>
       <c r="E89" s="22"/>
       <c r="F89" s="18" t="s">
         <v>11</v>
@@ -3005,17 +2959,15 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C90" s="22" t="n">
         <v>86</v>
       </c>
-      <c r="D90" s="22" t="s">
-        <v>107</v>
-      </c>
+      <c r="D90" s="22"/>
       <c r="E90" s="22"/>
       <c r="F90" s="18" t="s">
         <v>11</v>
@@ -3032,10 +2984,10 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C91" s="17" t="n">
         <v>28</v>
@@ -3057,10 +3009,10 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C92" s="17" t="n">
         <v>40</v>
@@ -3084,10 +3036,10 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C93" s="17" t="n">
         <v>31</v>
@@ -3109,10 +3061,10 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C94" s="17" t="n">
         <v>45</v>
@@ -3136,10 +3088,10 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C95" s="17" t="n">
         <v>40</v>
@@ -3161,10 +3113,10 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C96" s="17" t="n">
         <v>62</v>
@@ -3188,10 +3140,10 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C97" s="17" t="n">
         <v>51</v>
@@ -3213,10 +3165,10 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C98" s="17" t="n">
         <v>80</v>
@@ -3240,10 +3192,10 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C99" s="3" t="n">
         <v>159</v>
@@ -3267,10 +3219,10 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C100" s="3" t="n">
         <v>193</v>
@@ -3296,10 +3248,10 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="22"/>
@@ -3321,10 +3273,10 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C102" s="15" t="n">
         <v>333</v>
@@ -3348,10 +3300,10 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C103" s="17" t="n">
         <v>512</v>
@@ -3375,10 +3327,10 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C104" s="17" t="n">
         <v>606</v>

</xml_diff>